<commit_message>
Minor refinement of the spreadsheets
</commit_message>
<xml_diff>
--- a/cptVSsd_cpt.xlsx
+++ b/cptVSsd_cpt.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Trie Node Number</t>
   </si>
@@ -92,12 +92,6 @@
     <t>SD_CPT Time per query (s)</t>
   </si>
   <si>
-    <t>SD/CDS space</t>
-  </si>
-  <si>
-    <t>CPT/CDS space</t>
-  </si>
-  <si>
     <t>Trie Node Number with Dictionary</t>
   </si>
   <si>
@@ -110,22 +104,7 @@
     <t>CPT+ Time per query (s)</t>
   </si>
   <si>
-    <t>CPT+/CDS space</t>
-  </si>
-  <si>
-    <t>SD_CPT / CPT+ Time</t>
-  </si>
-  <si>
-    <t>II /CDS</t>
-  </si>
-  <si>
-    <t>SD_II / CDS</t>
-  </si>
-  <si>
     <t>CDS MB *</t>
-  </si>
-  <si>
-    <t>* CDS refers to Compact Dataset Size; depicts the estimated binary size of a dataset</t>
   </si>
   <si>
     <t>SD_Tree MB **</t>
@@ -134,7 +113,37 @@
     <t>II (SD-nodeNumber) MB **</t>
   </si>
   <si>
-    <t>** These fields are refering to the succinct representation of CPT+. Succinct data structures are used</t>
+    <t>* CDS refers to Compact Dataset Size; depicts the estimated binary size of a dataset in the disk</t>
+  </si>
+  <si>
+    <t>Ratio of SD_CPT over CPT+ Time</t>
+  </si>
+  <si>
+    <t>Ratio of CPT over CDS space</t>
+  </si>
+  <si>
+    <t>Ratio of CPT+ over CDS space</t>
+  </si>
+  <si>
+    <t>Ratio of II over CDS</t>
+  </si>
+  <si>
+    <t>Ratio of SD_II over CDS</t>
+  </si>
+  <si>
+    <t>II (SD-nodeNumber) Note:</t>
+  </si>
+  <si>
+    <t>II is built on node number of the SD_Tree; This means that instead of using a sequence index as a column, we use the node index that a sequence ends. Thus the LT is ommited in SD_CPT</t>
+  </si>
+  <si>
+    <t>During the develoment of succinct-CPT, we have came up with different names; Thus the names SD_CPT, cCPT, sCPT, succinctCPT, all refer to the same succinct implementation of CPT+ predictor and we have not fixed an "official" name yet</t>
+  </si>
+  <si>
+    <t>** These fields are refering to different data structure parts of the succinct representation of CPT+.</t>
+  </si>
+  <si>
+    <t>Ratio of SD_CPT over CDS space</t>
   </si>
 </sst>
 </file>
@@ -228,7 +237,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -239,6 +248,9 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -277,6 +289,2542 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Memory</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Utilised over Input size</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0522681703253885"/>
+          <c:y val="0.109028826226758"/>
+          <c:w val="0.928783067082751"/>
+          <c:h val="0.774654476155135"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ratio of SD_CPT over CDS space</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BMS1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BMS2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kosarak</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SIGN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BIBLE</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LEVIATHAN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MSNB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FIFA</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>NASA_08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>NASA_07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$19:$H$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.0429125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8483</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.89721052631579</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.30005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.586987012987012</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.726914285714286</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.177906896551724</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.133641025641026</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.707826666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.551146788990825</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ratio of CPT over CDS space</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BMS1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BMS2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kosarak</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SIGN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BIBLE</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LEVIATHAN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MSNB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FIFA</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>NASA_08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>NASA_07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$I$19:$I$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>40.962125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84.6718</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>179.2780701754386</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.73325</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58.57532467532467</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.462</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.773</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.80769230769231</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.48946666666667</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.46192660550459</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$J$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ratio of CPT+ over CDS space</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BMS1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BMS2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kosarak</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SIGN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BIBLE</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LEVIATHAN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MSNB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FIFA</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>NASA_08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>NASA_07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$19:$J$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>37.9605125</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80.335668</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>174.8126052631579</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>26.818075</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.22331818181817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>34.51742857142857</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.5127275862069</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20.32642564102564</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>56.273184</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.79121100917431</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="38955296"/>
+        <c:axId val="38961360"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="38955296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38961360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="38961360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38955296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Runtime per</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> query</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.399250211958331"/>
+          <c:y val="0.0241463366870123"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPT Time per query (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BMS1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BMS2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kosarak</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SIGN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BIBLE</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LEVIATHAN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MSNB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FIFA</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>NASA_08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>NASA_07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$2:$P$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0005263</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0548314</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0004902</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0170629</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0016166</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0101457</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0145394</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00238</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0035209</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CPT+ Time per query (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BMS1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BMS2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kosarak</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SIGN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BIBLE</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LEVIATHAN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MSNB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FIFA</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>NASA_08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>NASA_07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$2:$Q$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.000533984</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000645049</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.110252</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00104747</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.032386</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00357242</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0159825</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0263515</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.00458342</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.00657781</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SD_CPT Time per query (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>BMS1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>BMS2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Kosarak</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SIGN</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>BIBLE</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>LEVIATHAN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>MSNB</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>FIFA</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>NASA_08</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>NASA_07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$2:$R$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.000854</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000559</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.092288</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.001157</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.026142</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.003039</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.018703</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.025314</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.005649</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.007874</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="115"/>
+        <c:overlap val="-20"/>
+        <c:axId val="37115408"/>
+        <c:axId val="-50771472"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="37115408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-50771472"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-50771472"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="37115408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="222">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1177636</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>148550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>166768</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>115454</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>25657</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>25656</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>12827</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>153940</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,18 +3090,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S40"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="24.5" customWidth="1"/>
     <col min="2" max="3" width="24.1640625" customWidth="1"/>
     <col min="4" max="4" width="27.1640625" customWidth="1"/>
     <col min="5" max="5" width="34.6640625" customWidth="1"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
     <col min="8" max="8" width="27.5" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" customWidth="1"/>
     <col min="10" max="10" width="14.83203125" customWidth="1"/>
@@ -580,31 +3130,31 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>14</v>
@@ -616,13 +3166,13 @@
         <v>19</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -1225,23 +3775,23 @@
         <v>1.1970549468592131</v>
       </c>
     </row>
-    <row r="18" spans="8:15" x14ac:dyDescent="0.2">
-      <c r="H18" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>27</v>
+    <row r="18" spans="8:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="H18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" s="2" t="s">
-        <v>30</v>
+      <c r="M18" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N18" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="8:15" x14ac:dyDescent="0.2">
@@ -1529,18 +4079,32 @@
     <row r="30" spans="8:15" x14ac:dyDescent="0.2">
       <c r="O30" s="4"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>